<commit_message>
update sex ratio indicators and median_age
sex ratio for total age group and age between 0 to 1 year
and median_age are published in a 5 year interval. They
should have the freq dimension.
</commit_message>
<xml_diff>
--- a/etl/source/metadata.xlsx
+++ b/etl/source/metadata.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vagrant\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14715" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="New" sheetId="7" r:id="rId1"/>
@@ -15,20 +20,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">New!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="454">
   <si>
     <t>Total</t>
   </si>
@@ -1384,13 +1389,19 @@
   </si>
   <si>
     <t>_DependencyFormat</t>
+  </si>
+  <si>
+    <t>sex_ratio_at_birth</t>
+  </si>
+  <si>
+    <t>sex_ratio_total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1644,209 +1655,212 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="197">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="196" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2107,7 +2121,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2118,20 +2132,20 @@
   <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomRight" activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="60.1640625" customWidth="1"/>
+    <col min="1" max="1" width="60.125" customWidth="1"/>
     <col min="2" max="2" width="85.5" customWidth="1"/>
     <col min="3" max="3" width="49.5" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="6" width="18.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="5" max="6" width="18.125" customWidth="1"/>
+    <col min="7" max="7" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2159,62 +2173,65 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>264</v>
       </c>
       <c r="B2" t="s">
-        <v>286</v>
+        <v>344</v>
       </c>
       <c r="C2" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="D2" t="s">
-        <v>450</v>
+        <v>403</v>
       </c>
       <c r="E2" t="s">
         <v>398</v>
       </c>
       <c r="F2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>266</v>
       </c>
       <c r="B3" t="s">
-        <v>293</v>
+        <v>346</v>
       </c>
       <c r="C3" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="D3" t="s">
-        <v>451</v>
+        <v>403</v>
       </c>
       <c r="E3" t="s">
         <v>398</v>
       </c>
       <c r="F3" t="s">
-        <v>440</v>
+        <v>439</v>
+      </c>
+      <c r="G3" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>265</v>
       </c>
       <c r="B4" t="s">
-        <v>294</v>
+        <v>345</v>
       </c>
       <c r="C4" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="D4" t="s">
-        <v>451</v>
+        <v>403</v>
       </c>
       <c r="E4" t="s">
         <v>398</v>
       </c>
       <c r="F4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
@@ -2222,16 +2239,16 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>231</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E5" t="s">
         <v>398</v>
@@ -2239,74 +2256,71 @@
       <c r="F5" t="s">
         <v>440</v>
       </c>
-      <c r="G5" t="s">
-        <v>445</v>
-      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>264</v>
+        <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>344</v>
+        <v>293</v>
       </c>
       <c r="C6" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D6" t="s">
-        <v>403</v>
+        <v>451</v>
       </c>
       <c r="E6" t="s">
         <v>398</v>
       </c>
       <c r="F6" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>265</v>
+        <v>231</v>
       </c>
       <c r="B7" t="s">
-        <v>345</v>
+        <v>295</v>
       </c>
       <c r="C7" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D7" t="s">
-        <v>403</v>
+        <v>451</v>
       </c>
       <c r="E7" t="s">
         <v>398</v>
       </c>
       <c r="F7" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G7" t="s">
-        <v>1</v>
+        <v>445</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="B8" t="s">
-        <v>346</v>
+        <v>294</v>
       </c>
       <c r="C8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D8" t="s">
-        <v>403</v>
+        <v>451</v>
       </c>
       <c r="E8" t="s">
         <v>398</v>
       </c>
       <c r="F8" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G8" t="s">
-        <v>445</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2331,10 +2345,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B10" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C10" t="s">
         <v>381</v>
@@ -2349,15 +2363,15 @@
         <v>439</v>
       </c>
       <c r="G10" t="s">
-        <v>1</v>
+        <v>445</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C11" t="s">
         <v>381</v>
@@ -2372,7 +2386,7 @@
         <v>439</v>
       </c>
       <c r="G11" t="s">
-        <v>445</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2397,10 +2411,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B13" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C13" t="s">
         <v>381</v>
@@ -2415,15 +2429,15 @@
         <v>439</v>
       </c>
       <c r="G13" t="s">
-        <v>1</v>
+        <v>445</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C14" t="s">
         <v>381</v>
@@ -2438,7 +2452,7 @@
         <v>439</v>
       </c>
       <c r="G14" t="s">
-        <v>445</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2623,10 +2637,10 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>183</v>
+        <v>243</v>
       </c>
       <c r="B24" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C24" t="s">
         <v>388</v>
@@ -2639,6 +2653,9 @@
       </c>
       <c r="F24" t="s">
         <v>439</v>
+      </c>
+      <c r="G24" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2666,10 +2683,10 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>243</v>
+        <v>183</v>
       </c>
       <c r="B26" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C26" t="s">
         <v>388</v>
@@ -2683,45 +2700,45 @@
       <c r="F26" t="s">
         <v>439</v>
       </c>
-      <c r="G26" t="s">
-        <v>445</v>
-      </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B27" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C27" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D27" t="s">
         <v>217</v>
       </c>
       <c r="E27" t="s">
-        <v>397</v>
+        <v>449</v>
       </c>
       <c r="F27" t="s">
         <v>439</v>
+      </c>
+      <c r="G27" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B28" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C28" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D28" t="s">
         <v>217</v>
       </c>
       <c r="E28" t="s">
-        <v>397</v>
+        <v>449</v>
       </c>
       <c r="F28" t="s">
         <v>439</v>
@@ -2732,42 +2749,39 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
       <c r="B29" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C29" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D29" t="s">
         <v>217</v>
       </c>
       <c r="E29" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F29" t="s">
         <v>439</v>
-      </c>
-      <c r="G29" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B30" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C30" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D30" t="s">
         <v>217</v>
       </c>
       <c r="E30" t="s">
-        <v>449</v>
+        <v>397</v>
       </c>
       <c r="F30" t="s">
         <v>439</v>
@@ -2775,42 +2789,42 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B31" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C31" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="D31" t="s">
         <v>217</v>
       </c>
       <c r="E31" t="s">
-        <v>449</v>
+        <v>396</v>
       </c>
       <c r="F31" t="s">
         <v>439</v>
       </c>
       <c r="G31" t="s">
-        <v>1</v>
+        <v>445</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B32" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C32" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D32" t="s">
         <v>217</v>
       </c>
       <c r="E32" t="s">
-        <v>449</v>
+        <v>397</v>
       </c>
       <c r="F32" t="s">
         <v>439</v>
@@ -2821,10 +2835,10 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>204</v>
+        <v>234</v>
       </c>
       <c r="B33" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C33" t="s">
         <v>381</v>
@@ -2838,22 +2852,25 @@
       <c r="F33" t="s">
         <v>439</v>
       </c>
+      <c r="G33" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B34" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C34" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="D34" t="s">
         <v>217</v>
       </c>
       <c r="E34" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="F34" t="s">
         <v>439</v>
@@ -2864,25 +2881,22 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B35" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="C35" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="D35" t="s">
         <v>217</v>
       </c>
       <c r="E35" t="s">
-        <v>396</v>
+        <v>449</v>
       </c>
       <c r="F35" t="s">
         <v>439</v>
-      </c>
-      <c r="G35" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2947,30 +2961,33 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>164</v>
+        <v>245</v>
       </c>
       <c r="B39" t="s">
-        <v>341</v>
+        <v>316</v>
       </c>
       <c r="C39" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="D39" t="s">
         <v>214</v>
       </c>
       <c r="E39" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F39" t="s">
         <v>439</v>
+      </c>
+      <c r="G39" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B40" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C40" t="s">
         <v>389</v>
@@ -2985,47 +3002,44 @@
         <v>439</v>
       </c>
       <c r="G40" t="s">
-        <v>1</v>
+        <v>445</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>263</v>
+        <v>168</v>
       </c>
       <c r="B41" t="s">
-        <v>343</v>
+        <v>314</v>
       </c>
       <c r="C41" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="D41" t="s">
         <v>214</v>
       </c>
       <c r="E41" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F41" t="s">
         <v>439</v>
-      </c>
-      <c r="G41" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B42" t="s">
-        <v>314</v>
+        <v>341</v>
       </c>
       <c r="C42" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="D42" t="s">
         <v>214</v>
       </c>
       <c r="E42" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="F42" t="s">
         <v>439</v>
@@ -3056,33 +3070,33 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
       <c r="B44" t="s">
-        <v>316</v>
+        <v>342</v>
       </c>
       <c r="C44" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="D44" t="s">
         <v>214</v>
       </c>
       <c r="E44" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="F44" t="s">
         <v>439</v>
       </c>
       <c r="G44" t="s">
-        <v>445</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
       <c r="B45" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C45" t="s">
         <v>381</v>
@@ -3096,13 +3110,16 @@
       <c r="F45" t="s">
         <v>439</v>
       </c>
+      <c r="G45" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>254</v>
+        <v>165</v>
       </c>
       <c r="B46" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C46" t="s">
         <v>381</v>
@@ -3116,16 +3133,13 @@
       <c r="F46" t="s">
         <v>439</v>
       </c>
-      <c r="G46" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B47" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C47" t="s">
         <v>381</v>
@@ -3140,15 +3154,15 @@
         <v>439</v>
       </c>
       <c r="G47" t="s">
-        <v>445</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>257</v>
       </c>
       <c r="B48" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C48" t="s">
         <v>381</v>
@@ -3162,13 +3176,16 @@
       <c r="F48" t="s">
         <v>439</v>
       </c>
+      <c r="G48" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>256</v>
+        <v>166</v>
       </c>
       <c r="B49" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C49" t="s">
         <v>381</v>
@@ -3182,16 +3199,13 @@
       <c r="F49" t="s">
         <v>439</v>
       </c>
-      <c r="G49" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B50" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C50" t="s">
         <v>381</v>
@@ -3206,15 +3220,15 @@
         <v>439</v>
       </c>
       <c r="G50" t="s">
-        <v>445</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>167</v>
+        <v>259</v>
       </c>
       <c r="B51" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C51" t="s">
         <v>381</v>
@@ -3228,13 +3242,16 @@
       <c r="F51" t="s">
         <v>439</v>
       </c>
+      <c r="G51" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>258</v>
+        <v>167</v>
       </c>
       <c r="B52" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C52" t="s">
         <v>381</v>
@@ -3248,16 +3265,13 @@
       <c r="F52" t="s">
         <v>439</v>
       </c>
-      <c r="G52" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B53" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C53" t="s">
         <v>381</v>
@@ -3272,7 +3286,7 @@
         <v>439</v>
       </c>
       <c r="G53" t="s">
-        <v>445</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -3309,10 +3323,10 @@
         <v>416</v>
       </c>
       <c r="E55" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="F55" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -3457,10 +3471,10 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>188</v>
+        <v>233</v>
       </c>
       <c r="B63" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C63" t="s">
         <v>386</v>
@@ -3474,48 +3488,51 @@
       <c r="F63" t="s">
         <v>440</v>
       </c>
+      <c r="G63" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B64" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C64" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D64" t="s">
         <v>404</v>
       </c>
       <c r="E64" t="s">
-        <v>399</v>
+        <v>449</v>
       </c>
       <c r="F64" t="s">
         <v>440</v>
       </c>
       <c r="G64" t="s">
-        <v>1</v>
+        <v>445</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="B65" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="C65" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
       <c r="D65" t="s">
         <v>404</v>
       </c>
       <c r="E65" t="s">
-        <v>399</v>
+        <v>449</v>
       </c>
       <c r="F65" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G65" t="s">
         <v>445</v>
@@ -3523,10 +3540,10 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>191</v>
+        <v>270</v>
       </c>
       <c r="B66" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C66" t="s">
         <v>393</v>
@@ -3538,15 +3555,18 @@
         <v>397</v>
       </c>
       <c r="F66" t="s">
-        <v>440</v>
+        <v>439</v>
+      </c>
+      <c r="G66" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B67" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C67" t="s">
         <v>393</v>
@@ -3561,24 +3581,24 @@
         <v>440</v>
       </c>
       <c r="G67" t="s">
-        <v>1</v>
+        <v>445</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B68" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="C68" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D68" t="s">
         <v>404</v>
       </c>
       <c r="E68" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="F68" t="s">
         <v>440</v>
@@ -3589,42 +3609,45 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="B69" t="s">
-        <v>354</v>
+        <v>298</v>
       </c>
       <c r="C69" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="D69" t="s">
         <v>404</v>
       </c>
       <c r="E69" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F69" t="s">
-        <v>439</v>
+        <v>440</v>
+      </c>
+      <c r="G69" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="B70" t="s">
-        <v>355</v>
+        <v>288</v>
       </c>
       <c r="C70" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="D70" t="s">
         <v>404</v>
       </c>
       <c r="E70" t="s">
-        <v>397</v>
+        <v>449</v>
       </c>
       <c r="F70" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G70" t="s">
         <v>1</v>
@@ -3632,62 +3655,65 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B71" t="s">
-        <v>356</v>
+        <v>288</v>
       </c>
       <c r="C71" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D71" t="s">
         <v>404</v>
       </c>
       <c r="E71" t="s">
-        <v>397</v>
+        <v>449</v>
       </c>
       <c r="F71" t="s">
         <v>439</v>
       </c>
       <c r="G71" t="s">
-        <v>445</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>186</v>
+        <v>269</v>
       </c>
       <c r="B72" t="s">
-        <v>287</v>
+        <v>355</v>
       </c>
       <c r="C72" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="D72" t="s">
         <v>404</v>
       </c>
       <c r="E72" t="s">
-        <v>449</v>
+        <v>397</v>
       </c>
       <c r="F72" t="s">
-        <v>440</v>
+        <v>439</v>
+      </c>
+      <c r="G72" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>226</v>
+        <v>275</v>
       </c>
       <c r="B73" t="s">
-        <v>288</v>
+        <v>355</v>
       </c>
       <c r="C73" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="D73" t="s">
         <v>404</v>
       </c>
       <c r="E73" t="s">
-        <v>449</v>
+        <v>397</v>
       </c>
       <c r="F73" t="s">
         <v>440</v>
@@ -3698,56 +3724,56 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="B74" t="s">
-        <v>289</v>
+        <v>348</v>
       </c>
       <c r="C74" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="D74" t="s">
         <v>404</v>
       </c>
       <c r="E74" t="s">
-        <v>449</v>
+        <v>400</v>
       </c>
       <c r="F74" t="s">
         <v>440</v>
       </c>
       <c r="G74" t="s">
-        <v>445</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B75" t="s">
-        <v>357</v>
+        <v>297</v>
       </c>
       <c r="C75" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="D75" t="s">
         <v>404</v>
       </c>
       <c r="E75" t="s">
-        <v>449</v>
+        <v>399</v>
       </c>
       <c r="F75" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>271</v>
+        <v>186</v>
       </c>
       <c r="B76" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C76" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="D76" t="s">
         <v>404</v>
@@ -3756,99 +3782,87 @@
         <v>449</v>
       </c>
       <c r="F76" t="s">
-        <v>439</v>
-      </c>
-      <c r="G76" t="s">
-        <v>1</v>
+        <v>440</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>272</v>
+        <v>189</v>
       </c>
       <c r="B77" t="s">
-        <v>289</v>
+        <v>347</v>
       </c>
       <c r="C77" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D77" t="s">
         <v>404</v>
       </c>
       <c r="E77" t="s">
-        <v>449</v>
+        <v>400</v>
       </c>
       <c r="F77" t="s">
-        <v>439</v>
-      </c>
-      <c r="G77" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B78" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="C78" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="D78" t="s">
         <v>404</v>
       </c>
       <c r="E78" t="s">
-        <v>400</v>
+        <v>449</v>
       </c>
       <c r="F78" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>267</v>
+        <v>190</v>
       </c>
       <c r="B79" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="C79" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D79" t="s">
         <v>404</v>
       </c>
       <c r="E79" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F79" t="s">
-        <v>440</v>
-      </c>
-      <c r="G79" t="s">
-        <v>1</v>
+        <v>439</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>268</v>
+        <v>191</v>
       </c>
       <c r="B80" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="C80" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D80" t="s">
         <v>404</v>
       </c>
       <c r="E80" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F80" t="s">
         <v>440</v>
-      </c>
-      <c r="G80" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -3873,10 +3887,10 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>184</v>
+        <v>229</v>
       </c>
       <c r="B82" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C82" t="s">
         <v>384</v>
@@ -3890,16 +3904,19 @@
       <c r="F82" t="s">
         <v>440</v>
       </c>
+      <c r="G82" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>228</v>
+        <v>274</v>
       </c>
       <c r="B83" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C83" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="D83" t="s">
         <v>405</v>
@@ -3908,18 +3925,18 @@
         <v>449</v>
       </c>
       <c r="F83" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G83" t="s">
-        <v>1</v>
+        <v>445</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B84" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C84" t="s">
         <v>384</v>
@@ -3934,15 +3951,15 @@
         <v>440</v>
       </c>
       <c r="G84" t="s">
-        <v>445</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>185</v>
+        <v>273</v>
       </c>
       <c r="B85" t="s">
-        <v>358</v>
+        <v>291</v>
       </c>
       <c r="C85" t="s">
         <v>394</v>
@@ -3956,13 +3973,16 @@
       <c r="F85" t="s">
         <v>439</v>
       </c>
+      <c r="G85" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>273</v>
+        <v>185</v>
       </c>
       <c r="B86" t="s">
-        <v>291</v>
+        <v>358</v>
       </c>
       <c r="C86" t="s">
         <v>394</v>
@@ -3976,19 +3996,16 @@
       <c r="F86" t="s">
         <v>439</v>
       </c>
-      <c r="G86" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>274</v>
+        <v>184</v>
       </c>
       <c r="B87" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C87" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="D87" t="s">
         <v>405</v>
@@ -3997,10 +4014,7 @@
         <v>449</v>
       </c>
       <c r="F87" t="s">
-        <v>439</v>
-      </c>
-      <c r="G87" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -4125,39 +4139,39 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B94" t="s">
-        <v>359</v>
+        <v>281</v>
       </c>
       <c r="C94" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="D94" t="s">
-        <v>401</v>
+        <v>452</v>
       </c>
       <c r="E94" t="s">
-        <v>449</v>
+        <v>396</v>
       </c>
       <c r="F94" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B95" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="C95" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D95" t="s">
         <v>401</v>
       </c>
       <c r="E95" t="s">
-        <v>400</v>
+        <v>449</v>
       </c>
       <c r="F95" t="s">
         <v>440</v>
@@ -4165,16 +4179,16 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B96" t="s">
-        <v>281</v>
+        <v>351</v>
       </c>
       <c r="C96" t="s">
-        <v>381</v>
+        <v>392</v>
       </c>
       <c r="D96" t="s">
-        <v>401</v>
+        <v>453</v>
       </c>
       <c r="E96" t="s">
         <v>396</v>
@@ -4185,10 +4199,10 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>203</v>
+        <v>261</v>
       </c>
       <c r="B97" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C97" t="s">
         <v>389</v>
@@ -4202,13 +4216,16 @@
       <c r="F97" t="s">
         <v>439</v>
       </c>
+      <c r="G97" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>260</v>
+        <v>203</v>
       </c>
       <c r="B98" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C98" t="s">
         <v>389</v>
@@ -4222,16 +4239,13 @@
       <c r="F98" t="s">
         <v>439</v>
       </c>
-      <c r="G98" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B99" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C99" t="s">
         <v>389</v>
@@ -4246,7 +4260,7 @@
         <v>439</v>
       </c>
       <c r="G99" t="s">
-        <v>445</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -4371,10 +4385,10 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>206</v>
+        <v>247</v>
       </c>
       <c r="B106" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C106" t="s">
         <v>381</v>
@@ -4387,6 +4401,9 @@
       </c>
       <c r="F106" t="s">
         <v>439</v>
+      </c>
+      <c r="G106" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -4414,10 +4431,10 @@
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>247</v>
+        <v>206</v>
       </c>
       <c r="B108" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C108" t="s">
         <v>381</v>
@@ -4430,9 +4447,6 @@
       </c>
       <c r="F108" t="s">
         <v>439</v>
-      </c>
-      <c r="G108" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -4457,10 +4471,10 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110" t="s">
-        <v>208</v>
+        <v>249</v>
       </c>
       <c r="B110" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C110" t="s">
         <v>381</v>
@@ -4473,6 +4487,9 @@
       </c>
       <c r="F110" t="s">
         <v>439</v>
+      </c>
+      <c r="G110" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -4500,10 +4517,10 @@
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>249</v>
+        <v>208</v>
       </c>
       <c r="B112" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C112" t="s">
         <v>381</v>
@@ -4516,15 +4533,12 @@
       </c>
       <c r="F112" t="s">
         <v>439</v>
-      </c>
-      <c r="G112" t="s">
-        <v>445</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1">
     <sortState ref="A2:G112">
-      <sortCondition ref="D1:D112"/>
+      <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4542,13 +4556,13 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="64.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4729,9 +4743,9 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4917,14 +4931,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>